<commit_message>
got information out of excel and into python form using pandas
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8d3165a593c684c/Desktop/Winter Term 2025/Python For Engineers/Shack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="425" documentId="11_F25DC773A252ABDACC10485F691D4EAA5ADE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A00FD90-CA5F-402E-937D-BAF767448583}"/>
+  <xr:revisionPtr revIDLastSave="431" documentId="11_F25DC773A252ABDACC10485F691D4EAA5ADE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19E6BD08-173F-45A1-A627-3B63B832FC8B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,9 +148,6 @@
     <t>whipping cream</t>
   </si>
   <si>
-    <t>Ingredients (g)</t>
-  </si>
-  <si>
     <t>Chef time (minutes)</t>
   </si>
   <si>
@@ -161,22 +158,17 @@
   </si>
   <si>
     <t>Selling Price ($)</t>
+  </si>
+  <si>
+    <t>Items</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -228,16 +220,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,8 +530,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>36</v>
+      <c r="A1" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -907,7 +897,7 @@
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15">
         <v>90</v>
       </c>
       <c r="C15">
@@ -933,7 +923,7 @@
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16">
         <v>0</v>
       </c>
       <c r="C16">
@@ -959,7 +949,7 @@
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17">
         <v>0</v>
       </c>
       <c r="C17">
@@ -985,7 +975,7 @@
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18">
         <v>0</v>
       </c>
       <c r="C18">
@@ -1011,7 +1001,7 @@
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
@@ -1037,7 +1027,7 @@
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20">
         <v>30</v>
       </c>
       <c r="C20">
@@ -1063,7 +1053,7 @@
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21">
         <v>15</v>
       </c>
       <c r="C21">
@@ -1086,10 +1076,10 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="4">
+      <c r="A22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22">
         <v>6</v>
       </c>
       <c r="C22">
@@ -1112,10 +1102,10 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="4">
+      <c r="A23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23">
         <v>3</v>
       </c>
       <c r="C23">
@@ -1138,10 +1128,10 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="4">
+      <c r="A24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24">
         <v>2</v>
       </c>
       <c r="C24">
@@ -1164,10 +1154,10 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="4">
+      <c r="A25" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25">
         <v>18</v>
       </c>
       <c r="C25">
@@ -1188,36 +1178,6 @@
       <c r="H25">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1278,7 +1238,7 @@
         <v>11339.8</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D36" si="0">B3/C3</f>
+        <f t="shared" ref="D3:D22" si="0">B3/C3</f>
         <v>3.6155840491013955E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tested random ingredient and menu item addition to confirm flexibility of menu items/ingredients
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8d3165a593c684c/Desktop/Winter Term 2025/Python For Engineers/Shack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="11_6825FEF5E85EE9D777F772F8B879739B816F7662" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E668EB7-7117-4121-B5BC-8B4033ED2400}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="11_6825FEF5E85EE9D777F772F8B879739B816F7662" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9872010-E8B0-4CA0-9B3B-7E09DE5A3DAA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>Waiter Hourly Wage $</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>Selling Price ($)</t>
+  </si>
+  <si>
+    <t>Random Ing</t>
+  </si>
+  <si>
+    <t>random item</t>
   </si>
 </sst>
 </file>
@@ -166,7 +172,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -211,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -241,11 +247,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC6C6C6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -290,8 +307,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -598,9 +621,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -611,9 +636,10 @@
     <col min="5" max="5" width="22.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>28</v>
       </c>
@@ -638,8 +664,11 @@
       <c r="H1" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>7</v>
       </c>
@@ -664,8 +693,11 @@
       <c r="H2" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
@@ -690,8 +722,11 @@
       <c r="H3" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>9</v>
       </c>
@@ -716,8 +751,11 @@
       <c r="H4" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
@@ -742,8 +780,11 @@
       <c r="H5" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="11">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
@@ -768,8 +809,11 @@
       <c r="H6" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
@@ -794,8 +838,11 @@
       <c r="H7" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
@@ -820,8 +867,11 @@
       <c r="H8" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>36</v>
       </c>
@@ -846,8 +896,11 @@
       <c r="H9" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
@@ -872,8 +925,11 @@
       <c r="H10" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>16</v>
       </c>
@@ -898,8 +954,11 @@
       <c r="H11" s="11">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
@@ -924,8 +983,11 @@
       <c r="H12" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -950,8 +1012,11 @@
       <c r="H13" s="11">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I13" s="11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>19</v>
       </c>
@@ -976,8 +1041,11 @@
       <c r="H14" s="11">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>20</v>
       </c>
@@ -1002,8 +1070,11 @@
       <c r="H15" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>21</v>
       </c>
@@ -1028,8 +1099,11 @@
       <c r="H16" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I16" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>23</v>
       </c>
@@ -1054,8 +1128,11 @@
       <c r="H17" s="11">
         <v>300</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>24</v>
       </c>
@@ -1080,8 +1157,11 @@
       <c r="H18" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I18" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>25</v>
       </c>
@@ -1106,8 +1186,11 @@
       <c r="H19" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I19" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>26</v>
       </c>
@@ -1132,8 +1215,11 @@
       <c r="H20" s="11">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I20" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>27</v>
       </c>
@@ -1158,109 +1244,153 @@
       <c r="H21" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
+      <c r="I21" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="3">
+        <v>23</v>
+      </c>
+      <c r="C22" s="3">
+        <v>400</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3">
+        <v>69</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B23" s="11">
         <v>6</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C23" s="11">
         <v>6</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D23" s="13">
         <v>6.5</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E23" s="11">
         <v>7</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F23" s="13">
         <v>5.5</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G23" s="11">
         <v>2</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H23" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
+      <c r="I23" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B24" s="11">
         <v>3</v>
-      </c>
-      <c r="C23" s="11">
-        <v>3</v>
-      </c>
-      <c r="D23" s="11">
-        <v>3</v>
-      </c>
-      <c r="E23" s="11">
-        <v>3</v>
-      </c>
-      <c r="F23" s="11">
-        <v>3</v>
-      </c>
-      <c r="G23" s="11">
-        <v>3</v>
-      </c>
-      <c r="H23" s="11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="11">
-        <v>2</v>
       </c>
       <c r="C24" s="11">
         <v>3</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="11">
+        <v>3</v>
+      </c>
+      <c r="E24" s="11">
+        <v>3</v>
+      </c>
+      <c r="F24" s="11">
+        <v>3</v>
+      </c>
+      <c r="G24" s="11">
+        <v>3</v>
+      </c>
+      <c r="H24" s="11">
+        <v>3</v>
+      </c>
+      <c r="I24" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="11">
+        <v>2</v>
+      </c>
+      <c r="C25" s="11">
+        <v>3</v>
+      </c>
+      <c r="D25" s="13">
         <v>1.5</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E25" s="11">
         <v>5</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F25" s="11">
         <v>2</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G25" s="13">
         <v>0.5</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H25" s="13">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
+      <c r="I25" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B26" s="11">
         <v>18</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C26" s="11">
         <v>18</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D26" s="11">
         <v>10</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E26" s="11">
         <v>22</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F26" s="11">
         <v>12</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G26" s="11">
         <v>8</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H26" s="11">
         <v>6</v>
+      </c>
+      <c r="I26" s="11">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -1273,10 +1403,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1613,8 +1743,23 @@
         <v>500</v>
       </c>
       <c r="D22" s="7">
-        <f t="shared" ref="D2:D22" si="1">B22/C22</f>
+        <f t="shared" ref="D22:D23" si="1">B22/C22</f>
         <v>0.01</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="3">
+        <v>20</v>
+      </c>
+      <c r="C23" s="3">
+        <v>4000</v>
+      </c>
+      <c r="D23" s="9">
+        <f t="shared" si="1"/>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resturant menu analysis working to calculate profit for all items.
</commit_message>
<xml_diff>
--- a/Input.xlsx
+++ b/Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8d3165a593c684c/Desktop/Winter Term 2025/Python For Engineers/Shack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="11_6825FEF5E85EE9D777F772F8B879739B816F7662" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9872010-E8B0-4CA0-9B3B-7E09DE5A3DAA}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="11_6825FEF5E85EE9D777F772F8B879739B816F7662" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2B676EB-12BE-41C1-BBC1-A1D13E235929}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>Waiter Hourly Wage $</t>
   </si>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t>pommes</t>
-  </si>
-  <si>
-    <t>whipping crème</t>
   </si>
   <si>
     <t>Chef time (minutes)</t>
@@ -623,8 +620,8 @@
   </sheetPr>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,7 +662,7 @@
         <v>35</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -872,8 +869,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>36</v>
+      <c r="A9" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B9" s="11">
         <v>0</v>
@@ -1250,7 +1247,7 @@
     </row>
     <row r="22" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="3">
         <v>23</v>
@@ -1279,7 +1276,7 @@
     </row>
     <row r="23" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="11">
         <v>6</v>
@@ -1308,7 +1305,7 @@
     </row>
     <row r="24" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="11">
         <v>3</v>
@@ -1337,7 +1334,7 @@
     </row>
     <row r="25" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="11">
         <v>2</v>
@@ -1366,7 +1363,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="11">
         <v>18</v>
@@ -1405,8 +1402,8 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1749,7 +1746,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="3">
         <v>20</v>

</xml_diff>